<commit_message>
REsults for leach vs O_bleach
</commit_message>
<xml_diff>
--- a/pyFiles/MPC/Results/LEACHvsBLEACHexcel.xlsx
+++ b/pyFiles/MPC/Results/LEACHvsBLEACHexcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\axkar1\Documents\GitProj\ThesisWorkCybercom-master\pyFiles\MPC\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A292DB29-60C4-4C97-88EF-D5EF8E29B9F5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA170A20-2918-4EB9-A2AC-3EDB3A972536}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{C2EDAFF6-B2BC-42A2-8C5E-8A1477ED5F32}"/>
+    <workbookView xWindow="5124" yWindow="720" windowWidth="17280" windowHeight="8964" xr2:uid="{C2EDAFF6-B2BC-42A2-8C5E-8A1477ED5F32}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
   <si>
     <t>LEACH</t>
   </si>
@@ -106,6 +106,51 @@
   </si>
   <si>
     <t>712499.2</t>
+  </si>
+  <si>
+    <t>spread</t>
+  </si>
+  <si>
+    <t>O_BLEACH</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>startNRJ</t>
+  </si>
+  <si>
+    <t>Runs</t>
+  </si>
+  <si>
+    <t>159, 316</t>
+  </si>
+  <si>
+    <t>159, 390</t>
+  </si>
+  <si>
+    <t>157, 238</t>
+  </si>
+  <si>
+    <t>157, 244</t>
+  </si>
+  <si>
+    <t>155, 648</t>
+  </si>
+  <si>
+    <t>155, 700</t>
+  </si>
+  <si>
+    <t>158, 451</t>
+  </si>
+  <si>
+    <t>158, 479</t>
+  </si>
+  <si>
+    <t>156, 711</t>
+  </si>
+  <si>
+    <t>156, 591</t>
   </si>
 </sst>
 </file>
@@ -460,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5853AFCF-FBC7-4742-8ABC-2931436D5A7E}">
-  <dimension ref="B1:F9"/>
+  <dimension ref="B1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -472,7 +517,7 @@
     <col min="6" max="6" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -489,12 +534,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>4</v>
       </c>
@@ -511,7 +556,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -522,7 +567,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>6</v>
       </c>
@@ -533,7 +578,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -544,7 +589,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>8</v>
       </c>
@@ -555,14 +600,152 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15">
+        <v>5742</v>
+      </c>
+      <c r="D15">
+        <v>5767</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16">
+        <v>6117</v>
+      </c>
+      <c r="D16">
+        <v>6132</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17">
+        <v>5961</v>
+      </c>
+      <c r="D17">
+        <v>5973</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G17" t="s">
+        <v>7</v>
+      </c>
+      <c r="H17">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18">
+        <v>5920</v>
+      </c>
+      <c r="D18">
+        <v>5898</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G18" t="s">
+        <v>7</v>
+      </c>
+      <c r="H18">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19">
+        <v>5706</v>
+      </c>
+      <c r="D19">
+        <v>5655</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G19" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>